<commit_message>
He añadido una línea al final
</commit_message>
<xml_diff>
--- a/DatosPoblacion.xlsx
+++ b/DatosPoblacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FCharte\Trabajo\Libros\Actuales\MAExcel2016\MAExcel2016\03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdiuja\Documents\GitHub\Prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,12 +30,12 @@
     <definedName name="Oceania">Global!$B$203:$G$225</definedName>
     <definedName name="Poblacion">Global!$A$2:$I$225</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="245">
   <si>
     <t>  Angola</t>
   </si>
@@ -767,12 +767,15 @@
   </si>
   <si>
     <t>Población media de estos países</t>
+  </si>
+  <si>
+    <t>Otro continente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1220,10 +1223,10 @@
   <sheetPr>
     <outlinePr applyStyles="1"/>
   </sheetPr>
-  <dimension ref="A1:I233"/>
+  <dimension ref="A1:I235"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="F231" sqref="F231"/>
+      <selection activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8495,6 +8498,11 @@
       <c r="E233" s="16"/>
       <c r="H233" s="19"/>
       <c r="I233" s="16"/>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>